<commit_message>
added and updated task 3,4 and 5
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070"/>
+    <workbookView windowWidth="19200" windowHeight="7070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
@@ -15,15 +15,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Name</t>
   </si>
   <si>
-    <t>Petchimuthu Maharajan</t>
-  </si>
-  <si>
-    <t>Employee No</t>
+    <t>Petchimuthu Maharajan (2597)</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Trainee Consultant - Oracle Technical</t>
   </si>
   <si>
     <t>Github Link</t>
@@ -86,6 +89,12 @@
     <t>Bi Report - RTF Template with EXCEL output</t>
   </si>
   <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>Bi Report - Bursting</t>
+  </si>
+  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -153,6 +162,18 @@
   </si>
   <si>
     <t>Task 3&amp;4 completed</t>
+  </si>
+  <si>
+    <t>Task 3,4,5</t>
+  </si>
+  <si>
+    <t>Documentation</t>
+  </si>
+  <si>
+    <t>Bursting Concepts</t>
+  </si>
+  <si>
+    <t>Task 5 completed</t>
   </si>
 </sst>
 </file>
@@ -160,10 +181,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="29">
@@ -235,6 +256,14 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -242,28 +271,44 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -277,18 +322,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -308,68 +353,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,25 +423,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -432,13 +519,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -450,139 +585,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,6 +743,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -779,36 +830,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -822,152 +843,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -991,7 +1012,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1265,10 +1285,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -1301,42 +1321,42 @@
       <c r="B4" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="12">
-        <v>2597</v>
+      <c r="C4" s="12" t="s">
+        <v>3</v>
       </c>
       <c r="D4"/>
     </row>
     <row r="5" customHeight="1" spans="2:4">
       <c r="B5" s="11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5"/>
     </row>
     <row r="6" customHeight="1" spans="1:4">
       <c r="A6" s="14"/>
       <c r="B6" s="15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6" s="16" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" customHeight="1" spans="2:4">
       <c r="B7" s="17" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8" customHeight="1" spans="2:4">
       <c r="B8"/>
-      <c r="C8" s="19"/>
+      <c r="C8" s="14"/>
       <c r="D8"/>
     </row>
     <row r="9" customHeight="1" spans="2:4">
@@ -1344,82 +1364,105 @@
       <c r="D9"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="20" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="21" t="s">
+      <c r="A10" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="B10" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="C10" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="D10" s="20" t="s">
         <v>13</v>
       </c>
+      <c r="E10" s="21" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
-      <c r="A11" s="23" t="s">
-        <v>14</v>
+      <c r="A11" s="22" t="s">
+        <v>15</v>
       </c>
       <c r="B11" s="7">
         <v>44363</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>15</v>
+      <c r="C11" s="22" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="7">
         <v>44369</v>
       </c>
-      <c r="E11" s="23" t="s">
-        <v>16</v>
+      <c r="E11" s="22" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="23" t="s">
-        <v>17</v>
+      <c r="A12" s="22" t="s">
+        <v>18</v>
       </c>
       <c r="B12" s="7">
         <v>44364</v>
       </c>
-      <c r="C12" s="23" t="s">
-        <v>18</v>
+      <c r="C12" s="22" t="s">
+        <v>19</v>
       </c>
       <c r="D12" s="7">
         <v>44365</v>
       </c>
-      <c r="E12" s="23" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:4">
+      <c r="E12" s="22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:5">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>44370</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1">
         <v>44370</v>
       </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:4">
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:5">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>44370</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D14" s="1">
         <v>44370</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:5">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1">
+        <v>44371</v>
+      </c>
+      <c r="C15" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="1">
+        <v>44371</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1436,13 +1479,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="6" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="7" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="14.4272727272727" style="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
@@ -1452,19 +1495,19 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -1472,16 +1515,16 @@
         <v>44363</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -1489,16 +1532,16 @@
         <v>44364</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
@@ -1506,16 +1549,16 @@
         <v>44365</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
@@ -1523,33 +1566,33 @@
         <v>44368</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="1">
-        <v>44370</v>
+        <v>44369</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
@@ -1557,16 +1600,33 @@
         <v>44370</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" spans="1:5">
+      <c r="A8" s="1">
+        <v>44371</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added task 6 and 7
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -4,18 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="7070"/>
   </bookViews>
   <sheets>
-    <sheet name="SUMMARY" sheetId="1" r:id="rId1"/>
-    <sheet name="DAILY UPDATES" sheetId="2" r:id="rId2"/>
+    <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Daily Updates" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>Name</t>
   </si>
@@ -95,6 +95,18 @@
     <t>Bi Report - Bursting</t>
   </si>
   <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>Bi Report - Parameters and Multiple Sheet</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>Security Console</t>
+  </si>
+  <si>
     <t>DATE</t>
   </si>
   <si>
@@ -174,6 +186,27 @@
   </si>
   <si>
     <t>Task 5 completed</t>
+  </si>
+  <si>
+    <t>Nil</t>
+  </si>
+  <si>
+    <t>Bursting and Column Links</t>
+  </si>
+  <si>
+    <t>ESS jobs</t>
+  </si>
+  <si>
+    <t>Bi topics Revised</t>
+  </si>
+  <si>
+    <t>Task 6,7</t>
+  </si>
+  <si>
+    <t>Multiple Sheets</t>
+  </si>
+  <si>
+    <t>Task 6,7 competed</t>
   </si>
 </sst>
 </file>
@@ -181,10 +214,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="29">
@@ -260,6 +293,59 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -268,8 +354,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -284,21 +387,26 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -306,76 +414,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -388,13 +428,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -423,187 +456,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -744,21 +777,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
@@ -821,6 +839,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -843,152 +876,152 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -997,6 +1030,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1285,10 +1321,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -1300,7 +1336,7 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
-      <c r="A1" s="8"/>
+      <c r="A1" s="9"/>
       <c r="B1"/>
       <c r="D1"/>
     </row>
@@ -1309,54 +1345,54 @@
       <c r="D2"/>
     </row>
     <row r="3" customHeight="1" spans="2:4">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
       <c r="D3"/>
     </row>
     <row r="4" customHeight="1" spans="2:4">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>3</v>
       </c>
       <c r="D4"/>
     </row>
     <row r="5" customHeight="1" spans="2:4">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>5</v>
       </c>
       <c r="D5"/>
     </row>
     <row r="6" customHeight="1" spans="1:4">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="15"/>
+      <c r="B6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" customHeight="1" spans="2:4">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="19" t="s">
         <v>9</v>
       </c>
       <c r="D7"/>
     </row>
     <row r="8" customHeight="1" spans="2:4">
       <c r="B8"/>
-      <c r="C8" s="14"/>
+      <c r="C8" s="15"/>
       <c r="D8"/>
     </row>
     <row r="9" customHeight="1" spans="2:4">
@@ -1364,53 +1400,53 @@
       <c r="D9"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
-      <c r="A11" s="22" t="s">
+      <c r="A11" s="23" t="s">
         <v>15</v>
       </c>
       <c r="B11" s="7">
         <v>44363</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="23" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="7">
         <v>44369</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="23" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="23" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="7">
         <v>44364</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="23" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="7">
         <v>44365</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="23" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1462,6 +1498,40 @@
         <v>44371</v>
       </c>
       <c r="E15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:5">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1">
+        <v>44372</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1">
+        <v>44375</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" customHeight="1" spans="1:5">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="1">
+        <v>44372</v>
+      </c>
+      <c r="C17" t="s">
+        <v>29</v>
+      </c>
+      <c r="D17" s="1">
+        <v>44375</v>
+      </c>
+      <c r="E17" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1479,13 +1549,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelRow="7" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="14.4272727272727" style="1"/>
     <col min="3" max="3" width="32" customWidth="1"/>
@@ -1495,19 +1565,19 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -1515,16 +1585,16 @@
         <v>44363</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -1535,13 +1605,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
@@ -1549,16 +1619,16 @@
         <v>44365</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
@@ -1569,13 +1639,13 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
@@ -1586,13 +1656,13 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
@@ -1600,16 +1670,16 @@
         <v>44370</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -1617,16 +1687,50 @@
         <v>44371</v>
       </c>
       <c r="B8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" spans="1:5">
+      <c r="A9" s="1">
+        <v>44372</v>
+      </c>
+      <c r="B9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" spans="1:5">
+      <c r="A10" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" t="s">
+        <v>62</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added task 11 and 12
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="94">
   <si>
     <t>Name</t>
   </si>
@@ -125,6 +125,18 @@
     <t>Bi - Record limit in RTF</t>
   </si>
   <si>
+    <t>Task 11</t>
+  </si>
+  <si>
+    <t>Bi - Purchase Order Detailed Report</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>SQL - Joins, Set Operators and Functions</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -258,6 +270,33 @@
   </si>
   <si>
     <t>Revised and documented</t>
+  </si>
+  <si>
+    <t>FSD analysis</t>
+  </si>
+  <si>
+    <t>Table and Column identification</t>
+  </si>
+  <si>
+    <t>Task 11 analysed</t>
+  </si>
+  <si>
+    <t>Creation of data model</t>
+  </si>
+  <si>
+    <t>Generating EXCEL template</t>
+  </si>
+  <si>
+    <t>Task 11 template generated</t>
+  </si>
+  <si>
+    <t>Properties - Data Model and Report</t>
+  </si>
+  <si>
+    <t>SQL Documentation</t>
+  </si>
+  <si>
+    <t>Task 12 completed</t>
   </si>
 </sst>
 </file>
@@ -265,11 +304,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -338,7 +377,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,6 +390,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Arial"/>
@@ -359,23 +413,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -389,6 +429,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -436,14 +484,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
       <name val="Arial"/>
       <charset val="0"/>
@@ -451,7 +491,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,20 +512,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -507,187 +546,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -827,17 +866,31 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -881,15 +934,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -905,182 +949,177 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="29" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1372,10 +1411,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -1637,6 +1676,34 @@
         <v>17</v>
       </c>
     </row>
+    <row r="21" customHeight="1" spans="1:3">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" s="1">
+        <v>44379</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:5">
+      <c r="A22" t="s">
+        <v>38</v>
+      </c>
+      <c r="B22" s="1">
+        <v>44383</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1">
+        <v>44383</v>
+      </c>
+      <c r="E22" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" display="https://github.com/PETCHIMUTHU-M/fusion"/>
@@ -1651,10 +1718,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -1667,19 +1734,19 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -1687,16 +1754,16 @@
         <v>44363</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -1707,13 +1774,13 @@
         <v>18</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
@@ -1721,16 +1788,16 @@
         <v>44365</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
@@ -1741,13 +1808,13 @@
         <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
@@ -1758,13 +1825,13 @@
         <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
@@ -1772,16 +1839,16 @@
         <v>44370</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -1789,16 +1856,16 @@
         <v>44371</v>
       </c>
       <c r="B8" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
@@ -1806,16 +1873,16 @@
         <v>44372</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="D9" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="E9" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
@@ -1823,16 +1890,16 @@
         <v>44375</v>
       </c>
       <c r="B10" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
@@ -1840,16 +1907,16 @@
         <v>44376</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
@@ -1857,16 +1924,16 @@
         <v>44377</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="C12" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="E12" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
@@ -1874,16 +1941,67 @@
         <v>44378</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:5">
+      <c r="A14" s="1">
+        <v>44379</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" t="s">
+        <v>85</v>
+      </c>
+      <c r="D14" t="s">
+        <v>86</v>
+      </c>
+      <c r="E14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" customHeight="1" spans="1:5">
+      <c r="A15" s="1">
+        <v>44382</v>
+      </c>
+      <c r="B15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" t="s">
+        <v>89</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" customHeight="1" spans="1:5">
+      <c r="A16" s="1">
+        <v>44383</v>
+      </c>
+      <c r="B16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added tasks and docs
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="148">
   <si>
     <t>Name</t>
   </si>
@@ -155,6 +155,30 @@
     <t>Bi - Report Properties</t>
   </si>
   <si>
+    <t>Task 16</t>
+  </si>
+  <si>
+    <t>Bi - SCM Reports</t>
+  </si>
+  <si>
+    <t>Task 17</t>
+  </si>
+  <si>
+    <t>Bi - AP Aging report</t>
+  </si>
+  <si>
+    <t>Task 18</t>
+  </si>
+  <si>
+    <t>Bi - Ar Aging report</t>
+  </si>
+  <si>
+    <t>Task 19</t>
+  </si>
+  <si>
+    <t>Bi - Sales Order Detailed Report</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -339,6 +363,102 @@
   </si>
   <si>
     <t>Task 11,14 completed</t>
+  </si>
+  <si>
+    <t>Task 13,15</t>
+  </si>
+  <si>
+    <t>Documentation and SQL queries</t>
+  </si>
+  <si>
+    <t>Report properties</t>
+  </si>
+  <si>
+    <t>Documents updated</t>
+  </si>
+  <si>
+    <t>Documentation - Report properties</t>
+  </si>
+  <si>
+    <t>Task 15 documented</t>
+  </si>
+  <si>
+    <t>Report properties - Formatting</t>
+  </si>
+  <si>
+    <t>Report properties - Format mask</t>
+  </si>
+  <si>
+    <t>Document updated</t>
+  </si>
+  <si>
+    <t>SCM Reports - AP Invoice report</t>
+  </si>
+  <si>
+    <t>Task 16 completed</t>
+  </si>
+  <si>
+    <t>Analysed Ap Aging Report</t>
+  </si>
+  <si>
+    <t>Worked On Ap Aging Report</t>
+  </si>
+  <si>
+    <t>Task 17 analysed</t>
+  </si>
+  <si>
+    <t>Analysed Ar Aging Report</t>
+  </si>
+  <si>
+    <t>Worked On Ar Aging Report</t>
+  </si>
+  <si>
+    <t>Task 17 completed</t>
+  </si>
+  <si>
+    <t>Analysed Sales Order Report</t>
+  </si>
+  <si>
+    <t>Worked On Sales Order Report</t>
+  </si>
+  <si>
+    <t>Task 18 completed</t>
+  </si>
+  <si>
+    <t>Review on Ap aging report</t>
+  </si>
+  <si>
+    <t>Ap aging model query analysed</t>
+  </si>
+  <si>
+    <t>Model query analysed</t>
+  </si>
+  <si>
+    <t>Data model updation</t>
+  </si>
+  <si>
+    <t>Task 19 updated</t>
+  </si>
+  <si>
+    <t>Report generation</t>
+  </si>
+  <si>
+    <t>Task 19 completed</t>
+  </si>
+  <si>
+    <t>Task 18 updated</t>
+  </si>
+  <si>
+    <t>Task 19 analysed</t>
+  </si>
+  <si>
+    <t>Task 19 DM created</t>
+  </si>
+  <si>
+    <t>Sales Order Report Generated</t>
+  </si>
+  <si>
+    <t>Documentation for reports</t>
   </si>
 </sst>
 </file>
@@ -346,11 +466,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -418,6 +538,112 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -427,91 +653,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -526,7 +668,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -538,28 +680,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="36">
     <fill>
@@ -588,13 +708,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -606,169 +888,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -908,60 +1028,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -989,8 +1055,38 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1005,181 +1101,240 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="23" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="7" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1187,9 +1342,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1453,342 +1605,424 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E25"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
+    <col min="1" max="1" width="14.4272727272727" style="2"/>
     <col min="2" max="2" width="20.8636363636364" style="1" customWidth="1"/>
-    <col min="3" max="3" width="48.4545454545455" customWidth="1"/>
+    <col min="3" max="3" width="48.4545454545455" style="2" customWidth="1"/>
     <col min="4" max="4" width="19" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1363636363636" customWidth="1"/>
+    <col min="5" max="5" width="18.1363636363636" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="14.4272727272727" style="2"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:4">
-      <c r="A1" s="9"/>
-      <c r="B1"/>
-      <c r="D1"/>
+      <c r="A1" s="10"/>
+      <c r="B1" s="2"/>
+      <c r="D1" s="2"/>
     </row>
     <row r="2" customHeight="1" spans="2:4">
-      <c r="B2"/>
-      <c r="D2"/>
+      <c r="B2" s="2"/>
+      <c r="D2" s="2"/>
     </row>
     <row r="3" customHeight="1" spans="2:4">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3"/>
+      <c r="D3" s="2"/>
     </row>
     <row r="4" customHeight="1" spans="2:4">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D4"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" customHeight="1" spans="2:4">
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D5"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" customHeight="1" spans="1:4">
-      <c r="A6" s="15"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C6" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D6"/>
+      <c r="D6" s="2"/>
     </row>
     <row r="7" customHeight="1" spans="2:4">
-      <c r="B7" s="18" t="s">
+      <c r="B7" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D7"/>
+      <c r="D7" s="2"/>
     </row>
     <row r="8" customHeight="1" spans="2:4">
-      <c r="B8"/>
-      <c r="C8" s="15"/>
-      <c r="D8"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="2"/>
     </row>
     <row r="9" customHeight="1" spans="2:4">
-      <c r="B9"/>
-      <c r="D9"/>
+      <c r="B9" s="2"/>
+      <c r="D9" s="2"/>
     </row>
     <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="20" t="s">
+      <c r="A10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="21" t="s">
+      <c r="B10" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="23" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="7">
+      <c r="B11" s="8">
         <v>44363</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="8">
         <v>44369</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="7">
+      <c r="B12" s="8">
         <v>44364</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7">
+      <c r="D12" s="8">
         <v>44365</v>
       </c>
-      <c r="E12" s="23" t="s">
+      <c r="E12" s="6" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
       <c r="B13" s="1">
         <v>44370</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="1">
         <v>44370</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:5">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>44370</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="1">
         <v>44370</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:5">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="B15" s="1">
         <v>44371</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1">
         <v>44371</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
       <c r="B16" s="1">
         <v>44372</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="1">
         <v>44375</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>44372</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="1">
         <v>44375</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="1">
         <v>44375</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="1">
         <v>44376</v>
       </c>
-      <c r="E18" t="s">
+      <c r="E18" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
-      <c r="A19" t="s">
+      <c r="A19" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>44375</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="1">
         <v>44377</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:5">
-      <c r="A20" t="s">
+      <c r="A20" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B20" s="1">
         <v>44375</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D20" s="1">
         <v>44377</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:5">
-      <c r="A21" t="s">
+      <c r="A21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="B21" s="1">
         <v>44379</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="1">
         <v>44386</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>38</v>
       </c>
       <c r="B22" s="1">
         <v>44383</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="1">
         <v>44383</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" customHeight="1" spans="1:3">
-      <c r="A23" t="s">
+    <row r="23" customHeight="1" spans="1:5">
+      <c r="A23" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B23" s="1">
         <v>44383</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
+      <c r="D23" s="1">
+        <v>44410</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="24" customHeight="1" spans="1:5">
-      <c r="A24" t="s">
+      <c r="A24" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B24" s="1">
         <v>44386</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="1">
         <v>44386</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" customHeight="1" spans="1:3">
-      <c r="A25" t="s">
+    <row r="25" customHeight="1" spans="1:5">
+      <c r="A25" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B25" s="1">
         <v>44389</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
         <v>45</v>
+      </c>
+      <c r="D25" s="1">
+        <v>44393</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:5">
+      <c r="A26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="1">
+        <v>44392</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D26" s="1">
+        <v>44392</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:5">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1">
+        <v>44393</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="1">
+        <v>44396</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="1:5">
+      <c r="A28" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="1">
+        <v>44396</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D28" s="1">
+        <v>44397</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="1:5">
+      <c r="A29" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="1">
+        <v>44397</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="1">
+        <v>44398</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1805,346 +2039,615 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="14.4272727272727" style="1"/>
-    <col min="3" max="3" width="32" customWidth="1"/>
-    <col min="4" max="4" width="32.4272727272727" customWidth="1"/>
-    <col min="5" max="5" width="29.4272727272727" customWidth="1"/>
+    <col min="1" max="1" width="16.6363636363636" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.8181818181818" style="2" customWidth="1"/>
+    <col min="3" max="3" width="38.7272727272727" style="2" customWidth="1"/>
+    <col min="4" max="4" width="38.4545454545455" style="2" customWidth="1"/>
+    <col min="5" max="5" width="36.9090909090909" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="14.4272727272727" style="2"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
-      <c r="A1" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>49</v>
+      <c r="C1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
-      <c r="A2" s="4">
+      <c r="A2" s="5">
         <v>44363</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>53</v>
+      <c r="B2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
-      <c r="A3" s="4">
+      <c r="A3" s="5">
         <v>44364</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="E3" s="5" t="s">
-        <v>53</v>
+      <c r="C3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
-      <c r="A4" s="4">
+      <c r="A4" s="5">
         <v>44365</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>59</v>
+      <c r="B4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
-      <c r="A5" s="7">
+      <c r="A5" s="8">
         <v>44368</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" t="s">
-        <v>61</v>
-      </c>
-      <c r="E5" t="s">
-        <v>62</v>
+      <c r="C5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="1">
         <v>44369</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" t="s">
-        <v>64</v>
+      <c r="C6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
       <c r="A7" s="1">
         <v>44370</v>
       </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E7" t="s">
-        <v>68</v>
+      <c r="B7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
       <c r="A8" s="1">
         <v>44371</v>
       </c>
-      <c r="B8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>71</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
+      <c r="B8" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="1">
         <v>44372</v>
       </c>
-      <c r="B9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" t="s">
-        <v>75</v>
-      </c>
-      <c r="E9" t="s">
-        <v>76</v>
+      <c r="B9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
       <c r="A10" s="1">
         <v>44375</v>
       </c>
-      <c r="B10" t="s">
-        <v>77</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="B10" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
-        <v>78</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>79</v>
+      <c r="D10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
       <c r="A11" s="1">
         <v>44376</v>
       </c>
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-      <c r="C11" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" t="s">
-        <v>82</v>
-      </c>
-      <c r="E11" t="s">
-        <v>83</v>
+      <c r="B11" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
       <c r="A12" s="1">
         <v>44377</v>
       </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" t="s">
-        <v>85</v>
-      </c>
-      <c r="D12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12" t="s">
-        <v>87</v>
+      <c r="B12" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
       <c r="A13" s="1">
         <v>44378</v>
       </c>
-      <c r="B13" t="s">
-        <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>88</v>
-      </c>
-      <c r="D13" t="s">
-        <v>89</v>
-      </c>
-      <c r="E13" t="s">
-        <v>90</v>
+      <c r="B13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:5">
       <c r="A14" s="1">
         <v>44379</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D14" t="s">
-        <v>92</v>
-      </c>
-      <c r="E14" t="s">
-        <v>93</v>
+      <c r="C14" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:5">
       <c r="A15" s="1">
         <v>44382</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
-        <v>94</v>
-      </c>
-      <c r="D15" t="s">
-        <v>95</v>
-      </c>
-      <c r="E15" t="s">
-        <v>96</v>
+      <c r="C15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
       <c r="A16" s="1">
         <v>44383</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
-        <v>97</v>
-      </c>
-      <c r="D16" t="s">
-        <v>98</v>
-      </c>
-      <c r="E16" t="s">
-        <v>99</v>
+      <c r="C16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
       <c r="A17" s="1">
         <v>44384</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C17" t="s">
-        <v>100</v>
-      </c>
-      <c r="D17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E17" t="s">
-        <v>102</v>
+      <c r="C17" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
       <c r="A18" s="1">
         <v>44385</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C18" t="s">
-        <v>100</v>
-      </c>
-      <c r="D18" t="s">
-        <v>103</v>
-      </c>
-      <c r="E18" t="s">
-        <v>102</v>
+      <c r="C18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
       <c r="A19" s="1">
         <v>44386</v>
       </c>
-      <c r="B19" t="s">
-        <v>104</v>
-      </c>
-      <c r="C19" t="s">
-        <v>105</v>
-      </c>
-      <c r="D19" t="s">
-        <v>106</v>
-      </c>
-      <c r="E19" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="20" customHeight="1" spans="1:1">
+      <c r="B19" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" customHeight="1" spans="1:5">
       <c r="A20" s="1">
         <v>44389</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" customHeight="1" spans="1:5">
+      <c r="A21" s="1">
+        <v>44390</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" customHeight="1" spans="1:5">
+      <c r="A22" s="1">
+        <v>44391</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="23" customHeight="1" spans="1:5">
+      <c r="A23" s="1">
+        <v>44392</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" customHeight="1" spans="1:5">
+      <c r="A24" s="1">
+        <v>44393</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" customHeight="1" spans="1:5">
+      <c r="A25" s="1">
+        <v>44396</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="26" customHeight="1" spans="1:5">
+      <c r="A26" s="1">
+        <v>44397</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" customHeight="1" spans="1:5">
+      <c r="A27" s="1">
+        <v>44398</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="28" customHeight="1" spans="1:5">
+      <c r="A28" s="1">
+        <v>44399</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" customHeight="1" spans="1:5">
+      <c r="A29" s="1">
+        <v>44400</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="1:5">
+      <c r="A30" s="1">
+        <v>44403</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" customHeight="1" spans="1:5">
+      <c r="A31" s="1">
+        <v>44404</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="1:5">
+      <c r="A32" s="1">
+        <v>44405</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:5">
+      <c r="A33" s="1">
+        <v>44406</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" customHeight="1" spans="1:5">
+      <c r="A34" s="1">
+        <v>44407</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" customHeight="1" spans="1:5">
+      <c r="A35" s="1">
+        <v>44410</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added and modified tasks and docs
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -7,15 +7,15 @@
     <workbookView windowWidth="19200" windowHeight="7070"/>
   </bookViews>
   <sheets>
-    <sheet name="Summary" sheetId="1" r:id="rId1"/>
-    <sheet name="Daily Updates" sheetId="2" r:id="rId2"/>
+    <sheet name="Task Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Daily Tracker" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
   <si>
     <t>Name</t>
   </si>
@@ -47,6 +47,18 @@
     <t>Mohamedasifkhana Ahamedkabir</t>
   </si>
   <si>
+    <t>Mentor 3</t>
+  </si>
+  <si>
+    <t>Saravanan Kumarappa</t>
+  </si>
+  <si>
+    <t>Mentor 4</t>
+  </si>
+  <si>
+    <t>Benin Tharmalingam</t>
+  </si>
+  <si>
     <t>Task No</t>
   </si>
   <si>
@@ -179,6 +191,18 @@
     <t>Bi - Sales Order Detailed Report</t>
   </si>
   <si>
+    <t>Task 20</t>
+  </si>
+  <si>
+    <t>E-text - Citi Bank</t>
+  </si>
+  <si>
+    <t>Task 21</t>
+  </si>
+  <si>
+    <t>E-text - HDFC Bank</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -437,28 +461,121 @@
     <t>Data model updation</t>
   </si>
   <si>
+    <t>Task 17 updated</t>
+  </si>
+  <si>
+    <t>Report generation</t>
+  </si>
+  <si>
+    <t>Task 18 updated</t>
+  </si>
+  <si>
+    <t>Task 19 analysed</t>
+  </si>
+  <si>
+    <t>Task 19 DM created</t>
+  </si>
+  <si>
+    <t>Sales Order Report Generated</t>
+  </si>
+  <si>
+    <t>Documentation for reports</t>
+  </si>
+  <si>
     <t>Task 19 updated</t>
   </si>
   <si>
-    <t>Report generation</t>
-  </si>
-  <si>
-    <t>Task 19 completed</t>
-  </si>
-  <si>
-    <t>Task 18 updated</t>
-  </si>
-  <si>
-    <t>Task 19 analysed</t>
-  </si>
-  <si>
-    <t>Task 19 DM created</t>
-  </si>
-  <si>
-    <t>Sales Order Report Generated</t>
-  </si>
-  <si>
-    <t>Documentation for reports</t>
+    <t>Re-analysing Ap aging query</t>
+  </si>
+  <si>
+    <t>Query analysed and documented</t>
+  </si>
+  <si>
+    <t>Analyzing various tables in Ap aging query</t>
+  </si>
+  <si>
+    <t>Analyzing sub-queries in AP aging main query</t>
+  </si>
+  <si>
+    <t>Analyzing conditions and joins in AP aging query</t>
+  </si>
+  <si>
+    <t>Review on Ap Aging report</t>
+  </si>
+  <si>
+    <t>Ap Aging analysed</t>
+  </si>
+  <si>
+    <t>Type of Invoices</t>
+  </si>
+  <si>
+    <t>Accounting of Invoices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Accounts Payables </t>
+  </si>
+  <si>
+    <t>Accounts Payables</t>
+  </si>
+  <si>
+    <t>Analysing AP</t>
+  </si>
+  <si>
+    <t>Preparation for Review on Ap aging</t>
+  </si>
+  <si>
+    <t>Ap aging Review</t>
+  </si>
+  <si>
+    <t>Review completed</t>
+  </si>
+  <si>
+    <t>Analysing about XML and XPATH</t>
+  </si>
+  <si>
+    <t>Analysing e-text template format</t>
+  </si>
+  <si>
+    <t>Analysed</t>
+  </si>
+  <si>
+    <t>Creating sample E-text report</t>
+  </si>
+  <si>
+    <t>Discussion on Bank interface</t>
+  </si>
+  <si>
+    <t>Report created &amp; Files shared</t>
+  </si>
+  <si>
+    <t>E-text - FSD Analysis</t>
+  </si>
+  <si>
+    <t>E-text - Mapping doc Analysis</t>
+  </si>
+  <si>
+    <t>Task 20 analysed</t>
+  </si>
+  <si>
+    <t>Etext template creation</t>
+  </si>
+  <si>
+    <t>Template review</t>
+  </si>
+  <si>
+    <t>Task 20 template created</t>
+  </si>
+  <si>
+    <t>Template alteration</t>
+  </si>
+  <si>
+    <t>Sample output using BI Template Viewer</t>
+  </si>
+  <si>
+    <t>Citi Bank assignment completed</t>
+  </si>
+  <si>
+    <t>Template creation</t>
   </si>
 </sst>
 </file>
@@ -466,11 +583,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -541,21 +658,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
@@ -563,20 +665,27 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -593,6 +702,21 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -621,6 +745,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -629,24 +761,24 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -659,23 +791,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -708,55 +825,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -766,134 +1009,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="23">
     <border>
       <left/>
       <right/>
@@ -905,15 +1022,11 @@
       <left style="thin">
         <color auto="1"/>
       </left>
-      <right style="thin">
-        <color theme="4" tint="0.4"/>
-      </right>
+      <right/>
       <top style="thin">
         <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.4"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -933,12 +1046,21 @@
       <left style="thin">
         <color auto="1"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color theme="4" tint="0.4"/>
+        <color auto="1"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
       <bottom style="thin">
-        <color theme="4" tint="0.4"/>
+        <color theme="2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -954,6 +1076,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color theme="2"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color auto="1"/>
       </left>
@@ -962,6 +1108,17 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -986,7 +1143,7 @@
       </right>
       <top/>
       <bottom style="thin">
-        <color theme="4" tint="-0.5"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1028,11 +1185,41 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1057,21 +1244,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1102,192 +1274,177 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="24" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1296,7 +1453,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1317,31 +1474,36 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1605,10 +1767,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -1657,117 +1819,101 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" customHeight="1" spans="1:4">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17" t="s">
+    <row r="6" customHeight="1" spans="2:4">
+      <c r="B6" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" customHeight="1" spans="2:4">
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="18" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" customHeight="1" spans="2:4">
-      <c r="B8" s="2"/>
-      <c r="C8" s="16"/>
+    <row r="8" customHeight="1" spans="1:4">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>11</v>
+      </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9" customHeight="1" spans="2:4">
-      <c r="B9" s="2"/>
+      <c r="B9" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>13</v>
+      </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" customHeight="1" spans="1:5">
-      <c r="A10" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" s="23" t="s">
+    <row r="10" customHeight="1" spans="2:4">
+      <c r="B10" s="2"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" customHeight="1" spans="2:4">
+      <c r="B11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" customHeight="1" spans="1:5">
+      <c r="A12" s="24" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" customHeight="1" spans="1:5">
-      <c r="A11" s="6" t="s">
+      <c r="B12" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="8">
+      <c r="C12" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:5">
+      <c r="A13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="8">
         <v>44363</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="8">
+      <c r="C13" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="8">
         <v>44369</v>
       </c>
-      <c r="E11" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" customHeight="1" spans="1:5">
-      <c r="A12" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" s="8">
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" customHeight="1" spans="1:5">
+      <c r="A14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="8">
         <v>44364</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="8">
+      <c r="C14" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="8">
         <v>44365</v>
       </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="1">
-        <v>44370</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="E14" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="D13" s="1">
-        <v>44370</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="1:5">
-      <c r="A14" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="1">
-        <v>44370</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="1">
-        <v>44370</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:5">
@@ -1775,16 +1921,16 @@
         <v>24</v>
       </c>
       <c r="B15" s="1">
-        <v>44371</v>
+        <v>44370</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1">
-        <v>44371</v>
+        <v>44370</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
@@ -1792,16 +1938,16 @@
         <v>26</v>
       </c>
       <c r="B16" s="1">
-        <v>44372</v>
+        <v>44370</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="1">
-        <v>44375</v>
+        <v>44370</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
@@ -1809,16 +1955,16 @@
         <v>28</v>
       </c>
       <c r="B17" s="1">
-        <v>44372</v>
+        <v>44371</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="1">
-        <v>44375</v>
+        <v>44371</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
@@ -1826,16 +1972,16 @@
         <v>30</v>
       </c>
       <c r="B18" s="1">
-        <v>44375</v>
+        <v>44372</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D18" s="1">
-        <v>44376</v>
+        <v>44375</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
@@ -1843,16 +1989,16 @@
         <v>32</v>
       </c>
       <c r="B19" s="1">
-        <v>44375</v>
+        <v>44372</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D19" s="1">
-        <v>44377</v>
+        <v>44375</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:5">
@@ -1866,10 +2012,10 @@
         <v>35</v>
       </c>
       <c r="D20" s="1">
-        <v>44377</v>
+        <v>44376</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:5">
@@ -1877,16 +2023,16 @@
         <v>36</v>
       </c>
       <c r="B21" s="1">
-        <v>44379</v>
+        <v>44375</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D21" s="1">
-        <v>44386</v>
+        <v>44377</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
@@ -1894,16 +2040,16 @@
         <v>38</v>
       </c>
       <c r="B22" s="1">
-        <v>44383</v>
+        <v>44375</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>39</v>
       </c>
       <c r="D22" s="1">
-        <v>44383</v>
+        <v>44377</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:5">
@@ -1911,16 +2057,16 @@
         <v>40</v>
       </c>
       <c r="B23" s="1">
-        <v>44383</v>
+        <v>44379</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D23" s="1">
-        <v>44410</v>
+        <v>44386</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:5">
@@ -1928,16 +2074,16 @@
         <v>42</v>
       </c>
       <c r="B24" s="1">
-        <v>44386</v>
+        <v>44383</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D24" s="1">
-        <v>44386</v>
+        <v>44383</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:5">
@@ -1945,16 +2091,16 @@
         <v>44</v>
       </c>
       <c r="B25" s="1">
-        <v>44389</v>
+        <v>44383</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="1">
-        <v>44393</v>
+        <v>44405</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:5">
@@ -1962,16 +2108,16 @@
         <v>46</v>
       </c>
       <c r="B26" s="1">
-        <v>44392</v>
+        <v>44386</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>47</v>
       </c>
       <c r="D26" s="1">
-        <v>44392</v>
+        <v>44386</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:5">
@@ -1979,16 +2125,16 @@
         <v>48</v>
       </c>
       <c r="B27" s="1">
-        <v>44393</v>
+        <v>44389</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>49</v>
       </c>
       <c r="D27" s="1">
-        <v>44396</v>
+        <v>44393</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:5">
@@ -1996,16 +2142,16 @@
         <v>50</v>
       </c>
       <c r="B28" s="1">
-        <v>44396</v>
+        <v>44392</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>51</v>
       </c>
       <c r="D28" s="1">
-        <v>44397</v>
+        <v>44392</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:5">
@@ -2013,16 +2159,75 @@
         <v>52</v>
       </c>
       <c r="B29" s="1">
-        <v>44397</v>
+        <v>44393</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D29" s="1">
-        <v>44398</v>
+        <v>44404</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" customHeight="1" spans="1:5">
+      <c r="A30" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="1">
+        <v>44396</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="1">
+        <v>44405</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" customHeight="1" spans="1:5">
+      <c r="A31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" s="1">
+        <v>44397</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="1">
+        <v>44410</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" customHeight="1" spans="1:4">
+      <c r="A32" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="1">
+        <v>44424</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D32" s="1">
+        <v>44427</v>
+      </c>
+    </row>
+    <row r="33" customHeight="1" spans="1:3">
+      <c r="A33" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="1">
+        <v>44428</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2039,37 +2244,35 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="16.6363636363636" style="1" customWidth="1"/>
     <col min="2" max="2" width="16.8181818181818" style="2" customWidth="1"/>
-    <col min="3" max="3" width="38.7272727272727" style="2" customWidth="1"/>
-    <col min="4" max="4" width="38.4545454545455" style="2" customWidth="1"/>
-    <col min="5" max="5" width="36.9090909090909" style="2" customWidth="1"/>
+    <col min="3" max="5" width="39.4545454545455" style="2" customWidth="1"/>
     <col min="6" max="16384" width="14.4272727272727" style="2"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -2077,16 +2280,16 @@
         <v>44363</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -2094,16 +2297,16 @@
         <v>44364</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
@@ -2111,16 +2314,16 @@
         <v>44365</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
@@ -2128,16 +2331,16 @@
         <v>44368</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
@@ -2145,16 +2348,16 @@
         <v>44369</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
@@ -2162,16 +2365,16 @@
         <v>44370</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -2179,16 +2382,16 @@
         <v>44371</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
@@ -2196,16 +2399,16 @@
         <v>44372</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
@@ -2213,16 +2416,16 @@
         <v>44375</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
@@ -2230,16 +2433,16 @@
         <v>44376</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
@@ -2247,16 +2450,16 @@
         <v>44377</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
@@ -2264,16 +2467,16 @@
         <v>44378</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:5">
@@ -2281,16 +2484,16 @@
         <v>44379</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:5">
@@ -2298,16 +2501,16 @@
         <v>44382</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
@@ -2315,16 +2518,16 @@
         <v>44383</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
@@ -2332,16 +2535,16 @@
         <v>44384</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
@@ -2349,16 +2552,16 @@
         <v>44385</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
@@ -2366,16 +2569,16 @@
         <v>44386</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:5">
@@ -2383,16 +2586,16 @@
         <v>44389</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:5">
@@ -2400,16 +2603,16 @@
         <v>44390</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
@@ -2417,16 +2620,16 @@
         <v>44391</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:5">
@@ -2434,16 +2637,16 @@
         <v>44392</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:5">
@@ -2451,16 +2654,16 @@
         <v>44393</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:5">
@@ -2468,16 +2671,16 @@
         <v>44396</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:5">
@@ -2485,16 +2688,16 @@
         <v>44397</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:5">
@@ -2502,16 +2705,16 @@
         <v>44398</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:5">
@@ -2519,16 +2722,16 @@
         <v>44399</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:5">
@@ -2536,16 +2739,16 @@
         <v>44400</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:5">
@@ -2553,16 +2756,16 @@
         <v>44403</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:5">
@@ -2570,16 +2773,16 @@
         <v>44404</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:5">
@@ -2587,16 +2790,16 @@
         <v>44405</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:5">
@@ -2604,16 +2807,16 @@
         <v>44406</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:5">
@@ -2621,16 +2824,16 @@
         <v>44407</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
     </row>
     <row r="35" customHeight="1" spans="1:5">
@@ -2638,16 +2841,248 @@
         <v>44410</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" customHeight="1" spans="1:5">
+      <c r="A36" s="1">
+        <v>44411</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" customHeight="1" spans="1:5">
+      <c r="A37" s="1">
+        <v>44412</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="38" customHeight="1" spans="1:5">
+      <c r="A38" s="1">
+        <v>44413</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="39" customHeight="1" spans="1:5">
+      <c r="A39" s="1">
+        <v>44414</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="40" customHeight="1" spans="1:5">
+      <c r="A40" s="1">
+        <v>44417</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" customHeight="1" spans="1:5">
+      <c r="A41" s="1">
+        <v>44418</v>
+      </c>
+      <c r="B41" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>140</v>
+      <c r="C41" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" customHeight="1" spans="1:5">
+      <c r="A42" s="1">
+        <v>44419</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" customHeight="1" spans="1:5">
+      <c r="A43" s="1">
+        <v>44420</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="44" customHeight="1" spans="1:5">
+      <c r="A44" s="1">
+        <v>44421</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="45" customHeight="1" spans="1:5">
+      <c r="A45" s="1">
+        <v>44424</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" customHeight="1" spans="1:5">
+      <c r="A46" s="1">
+        <v>44425</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="47" customHeight="1" spans="1:5">
+      <c r="A47" s="1">
+        <v>44426</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="48" customHeight="1" spans="1:5">
+      <c r="A48" s="1">
+        <v>44427</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="49" customHeight="1" spans="1:3">
+      <c r="A49" s="1">
+        <v>44428</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>186</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added and updated tasks and docs
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070"/>
+    <workbookView windowWidth="19200" windowHeight="7070" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Task Summary" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="189">
   <si>
     <t>Name</t>
   </si>
@@ -576,6 +576,12 @@
   </si>
   <si>
     <t>Template creation</t>
+  </si>
+  <si>
+    <t>CitiBank Template alteration</t>
+  </si>
+  <si>
+    <t>Citi Bank assignment updated</t>
   </si>
 </sst>
 </file>
@@ -583,11 +589,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -663,29 +669,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF006100"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -707,8 +720,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -716,9 +730,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -731,31 +745,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -769,16 +759,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Arial"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -792,7 +798,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -825,187 +831,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1186,25 +1192,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1248,17 +1245,35 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1273,178 +1288,169 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1453,7 +1459,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1769,8 +1775,8 @@
   </sheetPr>
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -2216,7 +2222,7 @@
         <v>59</v>
       </c>
       <c r="D32" s="1">
-        <v>44427</v>
+        <v>44428</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:3">
@@ -2246,8 +2252,8 @@
   </sheetPr>
   <dimension ref="A1:E49"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -3074,7 +3080,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="49" customHeight="1" spans="1:3">
+    <row r="49" customHeight="1" spans="1:5">
       <c r="A49" s="1">
         <v>44428</v>
       </c>
@@ -3083,6 +3089,12 @@
       </c>
       <c r="C49" s="2" t="s">
         <v>186</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
created and altered folders and files
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -757,11 +757,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -830,15 +830,37 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -852,14 +874,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -867,28 +882,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -896,15 +889,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -919,15 +912,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -950,7 +935,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -959,14 +944,29 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -999,7 +999,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,73 +1041,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1089,13 +1053,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1113,13 +1077,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1131,55 +1161,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1359,13 +1359,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1394,30 +1413,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -1442,183 +1437,188 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="20" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1627,7 +1627,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="178" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2502,10 +2502,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E65"/>
+  <dimension ref="A1:E66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -3621,6 +3621,11 @@
         <v>244</v>
       </c>
     </row>
+    <row r="66" customHeight="1" spans="1:1">
+      <c r="A66" s="1">
+        <v>44454</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
added tasks and files
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="252">
   <si>
     <t>Name</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Trainee Consultant - Oracle Technical</t>
+    <t>Associate Consultant - Oracle Technical</t>
   </si>
   <si>
     <t>Github Link</t>
@@ -236,7 +236,13 @@
     <t>Task 27</t>
   </si>
   <si>
-    <t>E-text - CIMB Bank</t>
+    <t>E-text - CIMB Bank and WestPac Bank</t>
+  </si>
+  <si>
+    <t>Task 28</t>
+  </si>
+  <si>
+    <t>E-text - AmBank and MayBank</t>
   </si>
   <si>
     <t>Date</t>
@@ -740,9 +746,6 @@
     <t>Mapping Sheet created.</t>
   </si>
   <si>
-    <t>Task 28</t>
-  </si>
-  <si>
     <t>Template creation.</t>
   </si>
   <si>
@@ -750,6 +753,24 @@
   </si>
   <si>
     <t>Output generated</t>
+  </si>
+  <si>
+    <t>Analysing custom XML concepts</t>
+  </si>
+  <si>
+    <t>Review meet on Bank Payment</t>
+  </si>
+  <si>
+    <t>Review completed</t>
+  </si>
+  <si>
+    <t>PGP Keys</t>
+  </si>
+  <si>
+    <t>SSH Keys</t>
+  </si>
+  <si>
+    <t>PGP and SSH keys analysed</t>
   </si>
 </sst>
 </file>
@@ -757,11 +778,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -830,23 +851,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -859,15 +871,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF800080"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -882,22 +896,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -944,7 +943,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -959,7 +965,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -967,6 +980,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -999,7 +1020,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1011,43 +1044,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1065,13 +1062,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1083,7 +1134,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1095,19 +1146,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1119,7 +1164,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1131,55 +1188,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1360,16 +1381,31 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1389,21 +1425,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1413,17 +1434,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1431,8 +1461,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1447,178 +1477,169 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="6" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1627,7 +1648,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1941,10 +1962,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+      <selection activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -2477,7 +2498,7 @@
         <v>44448</v>
       </c>
     </row>
-    <row r="39" customHeight="1" spans="1:3">
+    <row r="39" customHeight="1" spans="1:4">
       <c r="A39" s="2" t="s">
         <v>72</v>
       </c>
@@ -2486,6 +2507,23 @@
       </c>
       <c r="C39" s="2" t="s">
         <v>73</v>
+      </c>
+      <c r="D39" s="1">
+        <v>44453</v>
+      </c>
+    </row>
+    <row r="40" customHeight="1" spans="1:4">
+      <c r="A40" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B40" s="1">
+        <v>44454</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="1">
+        <v>44455</v>
       </c>
     </row>
   </sheetData>
@@ -2502,10 +2540,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E66"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -2518,19 +2556,19 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -2538,16 +2576,16 @@
         <v>44363</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -2558,13 +2596,13 @@
         <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
@@ -2572,16 +2610,16 @@
         <v>44365</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
@@ -2592,13 +2630,13 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
@@ -2609,13 +2647,13 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
@@ -2623,16 +2661,16 @@
         <v>44370</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -2640,16 +2678,16 @@
         <v>44371</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
@@ -2657,16 +2695,16 @@
         <v>44372</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
@@ -2674,16 +2712,16 @@
         <v>44375</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
@@ -2691,16 +2729,16 @@
         <v>44376</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
@@ -2708,16 +2746,16 @@
         <v>44377</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
@@ -2725,16 +2763,16 @@
         <v>44378</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:5">
@@ -2745,13 +2783,13 @@
         <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:5">
@@ -2762,13 +2800,13 @@
         <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
@@ -2779,13 +2817,13 @@
         <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
@@ -2796,13 +2834,13 @@
         <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
@@ -2813,13 +2851,13 @@
         <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
@@ -2827,16 +2865,16 @@
         <v>44386</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:5">
@@ -2844,16 +2882,16 @@
         <v>44389</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:5">
@@ -2864,13 +2902,13 @@
         <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
@@ -2881,13 +2919,13 @@
         <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:5">
@@ -2898,13 +2936,13 @@
         <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:5">
@@ -2915,13 +2953,13 @@
         <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:5">
@@ -2932,13 +2970,13 @@
         <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:5">
@@ -2949,13 +2987,13 @@
         <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:5">
@@ -2966,13 +3004,13 @@
         <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:5">
@@ -2980,16 +3018,16 @@
         <v>44399</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:5">
@@ -2997,16 +3035,16 @@
         <v>44400</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:5">
@@ -3017,13 +3055,13 @@
         <v>52</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:5">
@@ -3034,13 +3072,13 @@
         <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:5">
@@ -3051,13 +3089,13 @@
         <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:5">
@@ -3068,13 +3106,13 @@
         <v>56</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:5">
@@ -3085,13 +3123,13 @@
         <v>56</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" customHeight="1" spans="1:5">
@@ -3102,13 +3140,13 @@
         <v>56</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:5">
@@ -3116,16 +3154,16 @@
         <v>44411</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="37" customHeight="1" spans="1:5">
@@ -3133,16 +3171,16 @@
         <v>44412</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" customHeight="1" spans="1:5">
@@ -3150,16 +3188,16 @@
         <v>44413</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="39" customHeight="1" spans="1:5">
@@ -3167,16 +3205,16 @@
         <v>44414</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" customHeight="1" spans="1:5">
@@ -3184,16 +3222,16 @@
         <v>44417</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="1:5">
@@ -3204,13 +3242,13 @@
         <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D41" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E41" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="1:5">
@@ -3221,13 +3259,13 @@
         <v>52</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" customHeight="1" spans="1:5">
@@ -3235,16 +3273,16 @@
         <v>44420</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
     </row>
     <row r="44" customHeight="1" spans="1:5">
@@ -3252,16 +3290,16 @@
         <v>44421</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" customHeight="1" spans="1:5">
@@ -3269,16 +3307,16 @@
         <v>44424</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
     </row>
     <row r="46" customHeight="1" spans="1:5">
@@ -3289,13 +3327,13 @@
         <v>58</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="1:5">
@@ -3306,13 +3344,13 @@
         <v>58</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="1:5">
@@ -3323,13 +3361,13 @@
         <v>58</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
     </row>
     <row r="49" customHeight="1" spans="1:5">
@@ -3340,13 +3378,13 @@
         <v>60</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" customHeight="1" spans="1:5">
@@ -3357,13 +3395,13 @@
         <v>60</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="51" customHeight="1" spans="1:5">
@@ -3374,13 +3412,13 @@
         <v>60</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="52" customHeight="1" spans="1:5">
@@ -3388,16 +3426,16 @@
         <v>44433</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D52" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="E52" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" customHeight="1" spans="1:5">
@@ -3408,13 +3446,13 @@
         <v>64</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" customHeight="1" spans="1:5">
@@ -3425,13 +3463,13 @@
         <v>64</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" customHeight="1" spans="1:5">
@@ -3442,13 +3480,13 @@
         <v>64</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
     </row>
     <row r="56" customHeight="1" spans="1:5">
@@ -3456,16 +3494,16 @@
         <v>44439</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="57" customHeight="1" spans="1:5">
@@ -3473,16 +3511,16 @@
         <v>44440</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" customHeight="1" spans="1:5">
@@ -3493,13 +3531,13 @@
         <v>66</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
     </row>
     <row r="59" customHeight="1" spans="1:5">
@@ -3510,13 +3548,13 @@
         <v>66</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
     </row>
     <row r="60" customHeight="1" spans="1:5">
@@ -3527,13 +3565,13 @@
         <v>66</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" customHeight="1" spans="1:5">
@@ -3544,13 +3582,13 @@
         <v>68</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
     </row>
     <row r="62" customHeight="1" spans="1:5">
@@ -3561,13 +3599,13 @@
         <v>68</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
     </row>
     <row r="63" customHeight="1" spans="1:5">
@@ -3578,13 +3616,13 @@
         <v>70</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
     </row>
     <row r="64" customHeight="1" spans="1:5">
@@ -3595,13 +3633,13 @@
         <v>72</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" customHeight="1" spans="1:5">
@@ -3609,21 +3647,84 @@
         <v>44453</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>241</v>
+        <v>72</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="66" customHeight="1" spans="1:1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="66" customHeight="1" spans="1:5">
       <c r="A66" s="1">
         <v>44454</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="67" customHeight="1" spans="1:5">
+      <c r="A67" s="1">
+        <v>44455</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="68" customHeight="1" spans="1:5">
+      <c r="A68" s="1">
+        <v>44456</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="69" customHeight="1" spans="1:5">
+      <c r="A69" s="1">
+        <v>44459</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added and updated tasks
</commit_message>
<xml_diff>
--- a/Fusion-Tracker.xlsx
+++ b/Fusion-Tracker.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070" activeTab="1"/>
+    <workbookView windowWidth="19200" windowHeight="7070"/>
   </bookViews>
   <sheets>
     <sheet name="Task Summary" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="259">
   <si>
     <t>Name</t>
   </si>
@@ -245,6 +245,18 @@
     <t>E-text - AmBank and MayBank</t>
   </si>
   <si>
+    <t>Task 29</t>
+  </si>
+  <si>
+    <t>PGP and SSH keys</t>
+  </si>
+  <si>
+    <t>Task 30</t>
+  </si>
+  <si>
+    <t>Bank Payment Technical Documentation</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
@@ -767,10 +779,19 @@
     <t>PGP Keys</t>
   </si>
   <si>
+    <t>PGP keys analysed</t>
+  </si>
+  <si>
     <t>SSH Keys</t>
   </si>
   <si>
-    <t>PGP and SSH keys analysed</t>
+    <t>SSH keys analysed</t>
+  </si>
+  <si>
+    <t>Partially completed</t>
+  </si>
+  <si>
+    <t>Documentation completed</t>
   </si>
 </sst>
 </file>
@@ -778,11 +799,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="[$-409]d/mmm/yyyy;@"/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="180" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="180" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="29">
     <font>
@@ -851,14 +872,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -871,9 +893,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -882,21 +939,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -914,14 +956,6 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Arial"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -956,13 +990,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -971,13 +998,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Arial"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Arial"/>
@@ -1020,6 +1041,102 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -1032,7 +1149,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1044,7 +1197,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1056,7 +1209,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1068,139 +1221,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1380,36 +1401,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1428,8 +1419,32 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1439,6 +1454,21 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1460,15 +1490,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1480,7 +1501,13 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1489,157 +1516,151 @@
     <xf numFmtId="179" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="18" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1648,7 +1669,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1962,10 +1983,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -2526,6 +2547,37 @@
         <v>44455</v>
       </c>
     </row>
+    <row r="41" customHeight="1" spans="1:4">
+      <c r="A41" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B41" s="1">
+        <v>44456</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="1">
+        <v>44460</v>
+      </c>
+    </row>
+    <row r="42" customHeight="1" spans="1:5">
+      <c r="A42" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B42" s="1">
+        <v>44456</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D42" s="1">
+        <v>44466</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1" display="https://github.com/PETCHIMUTHU-M/fusion"/>
@@ -2540,10 +2592,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E75" sqref="E75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4272727272727" defaultRowHeight="15.75" customHeight="1" outlineLevelCol="4"/>
@@ -2556,19 +2608,19 @@
   <sheetData>
     <row r="1" customHeight="1" spans="1:5">
       <c r="A1" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" customHeight="1" spans="1:5">
@@ -2576,16 +2628,16 @@
         <v>44363</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
@@ -2596,13 +2648,13 @@
         <v>22</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
@@ -2610,16 +2662,16 @@
         <v>44365</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
@@ -2630,13 +2682,13 @@
         <v>19</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
@@ -2647,13 +2699,13 @@
         <v>19</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
@@ -2661,16 +2713,16 @@
         <v>44370</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
@@ -2678,16 +2730,16 @@
         <v>44371</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
@@ -2695,16 +2747,16 @@
         <v>44372</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" customHeight="1" spans="1:5">
@@ -2712,16 +2764,16 @@
         <v>44375</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" customHeight="1" spans="1:5">
@@ -2729,16 +2781,16 @@
         <v>44376</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" customHeight="1" spans="1:5">
@@ -2746,16 +2798,16 @@
         <v>44377</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" customHeight="1" spans="1:5">
@@ -2763,16 +2815,16 @@
         <v>44378</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customHeight="1" spans="1:5">
@@ -2783,13 +2835,13 @@
         <v>40</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" customHeight="1" spans="1:5">
@@ -2800,13 +2852,13 @@
         <v>40</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="16" customHeight="1" spans="1:5">
@@ -2817,13 +2869,13 @@
         <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" customHeight="1" spans="1:5">
@@ -2834,13 +2886,13 @@
         <v>44</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" customHeight="1" spans="1:5">
@@ -2851,13 +2903,13 @@
         <v>44</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" customHeight="1" spans="1:5">
@@ -2865,16 +2917,16 @@
         <v>44386</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="20" customHeight="1" spans="1:5">
@@ -2882,16 +2934,16 @@
         <v>44389</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" customHeight="1" spans="1:5">
@@ -2902,13 +2954,13 @@
         <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" customHeight="1" spans="1:5">
@@ -2919,13 +2971,13 @@
         <v>48</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:5">
@@ -2936,13 +2988,13 @@
         <v>50</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:5">
@@ -2953,13 +3005,13 @@
         <v>52</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="25" customHeight="1" spans="1:5">
@@ -2970,13 +3022,13 @@
         <v>54</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="26" customHeight="1" spans="1:5">
@@ -2987,13 +3039,13 @@
         <v>56</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
     </row>
     <row r="27" customHeight="1" spans="1:5">
@@ -3004,13 +3056,13 @@
         <v>56</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D27" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>158</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="28" customHeight="1" spans="1:5">
@@ -3018,16 +3070,16 @@
         <v>44399</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="29" customHeight="1" spans="1:5">
@@ -3035,16 +3087,16 @@
         <v>44400</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" customHeight="1" spans="1:5">
@@ -3055,13 +3107,13 @@
         <v>52</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
     </row>
     <row r="31" customHeight="1" spans="1:5">
@@ -3072,13 +3124,13 @@
         <v>52</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" customHeight="1" spans="1:5">
@@ -3089,13 +3141,13 @@
         <v>54</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" customHeight="1" spans="1:5">
@@ -3106,13 +3158,13 @@
         <v>56</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" customHeight="1" spans="1:5">
@@ -3123,13 +3175,13 @@
         <v>56</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
     </row>
     <row r="35" customHeight="1" spans="1:5">
@@ -3140,13 +3192,13 @@
         <v>56</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" customHeight="1" spans="1:5">
@@ -3154,16 +3206,16 @@
         <v>44411</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" customHeight="1" spans="1:5">
@@ -3171,16 +3223,16 @@
         <v>44412</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="38" customHeight="1" spans="1:5">
@@ -3188,16 +3240,16 @@
         <v>44413</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="39" customHeight="1" spans="1:5">
@@ -3205,16 +3257,16 @@
         <v>44414</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
     </row>
     <row r="40" customHeight="1" spans="1:5">
@@ -3222,16 +3274,16 @@
         <v>44417</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" customHeight="1" spans="1:5">
@@ -3242,13 +3294,13 @@
         <v>52</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" customHeight="1" spans="1:5">
@@ -3259,13 +3311,13 @@
         <v>52</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
     </row>
     <row r="43" customHeight="1" spans="1:5">
@@ -3273,16 +3325,16 @@
         <v>44420</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
     </row>
     <row r="44" customHeight="1" spans="1:5">
@@ -3290,16 +3342,16 @@
         <v>44421</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
     </row>
     <row r="45" customHeight="1" spans="1:5">
@@ -3307,16 +3359,16 @@
         <v>44424</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
     </row>
     <row r="46" customHeight="1" spans="1:5">
@@ -3327,13 +3379,13 @@
         <v>58</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
     </row>
     <row r="47" customHeight="1" spans="1:5">
@@ -3344,13 +3396,13 @@
         <v>58</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
     </row>
     <row r="48" customHeight="1" spans="1:5">
@@ -3361,13 +3413,13 @@
         <v>58</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="49" customHeight="1" spans="1:5">
@@ -3378,13 +3430,13 @@
         <v>60</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
     </row>
     <row r="50" customHeight="1" spans="1:5">
@@ -3395,13 +3447,13 @@
         <v>60</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" customHeight="1" spans="1:5">
@@ -3412,13 +3464,13 @@
         <v>60</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
     </row>
     <row r="52" customHeight="1" spans="1:5">
@@ -3426,16 +3478,16 @@
         <v>44433</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" customHeight="1" spans="1:5">
@@ -3446,13 +3498,13 @@
         <v>64</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
     </row>
     <row r="54" customHeight="1" spans="1:5">
@@ -3463,13 +3515,13 @@
         <v>64</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
     </row>
     <row r="55" customHeight="1" spans="1:5">
@@ -3480,13 +3532,13 @@
         <v>64</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>216</v>
+        <v>220</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>217</v>
+        <v>221</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>218</v>
+        <v>222</v>
       </c>
     </row>
     <row r="56" customHeight="1" spans="1:5">
@@ -3494,16 +3546,16 @@
         <v>44439</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>219</v>
+        <v>223</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" customHeight="1" spans="1:5">
@@ -3511,16 +3563,16 @@
         <v>44440</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>222</v>
+        <v>226</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>223</v>
+        <v>227</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>224</v>
+        <v>228</v>
       </c>
     </row>
     <row r="58" customHeight="1" spans="1:5">
@@ -3531,13 +3583,13 @@
         <v>66</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>226</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" customHeight="1" spans="1:5">
@@ -3548,13 +3600,13 @@
         <v>66</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="60" customHeight="1" spans="1:5">
@@ -3565,13 +3617,13 @@
         <v>66</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>227</v>
+        <v>231</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>228</v>
+        <v>232</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>230</v>
+        <v>234</v>
       </c>
     </row>
     <row r="61" customHeight="1" spans="1:5">
@@ -3582,13 +3634,13 @@
         <v>68</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>231</v>
+        <v>235</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
     </row>
     <row r="62" customHeight="1" spans="1:5">
@@ -3599,13 +3651,13 @@
         <v>68</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" customHeight="1" spans="1:5">
@@ -3616,13 +3668,13 @@
         <v>70</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>239</v>
+        <v>243</v>
       </c>
     </row>
     <row r="64" customHeight="1" spans="1:5">
@@ -3633,13 +3685,13 @@
         <v>72</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="65" customHeight="1" spans="1:5">
@@ -3650,13 +3702,13 @@
         <v>72</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="66" customHeight="1" spans="1:5">
@@ -3667,13 +3719,13 @@
         <v>74</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>240</v>
+        <v>244</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>242</v>
+        <v>246</v>
       </c>
     </row>
     <row r="67" customHeight="1" spans="1:5">
@@ -3684,13 +3736,13 @@
         <v>74</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>243</v>
+        <v>247</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>244</v>
+        <v>248</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>245</v>
+        <v>249</v>
       </c>
     </row>
     <row r="68" customHeight="1" spans="1:5">
@@ -3698,16 +3750,16 @@
         <v>44456</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>246</v>
+        <v>250</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>248</v>
+        <v>252</v>
       </c>
     </row>
     <row r="69" customHeight="1" spans="1:5">
@@ -3715,16 +3767,101 @@
         <v>44459</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>103</v>
+        <v>76</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>249</v>
+        <v>253</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>251</v>
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" customHeight="1" spans="1:5">
+      <c r="A70" s="1">
+        <v>44460</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="71" customHeight="1" spans="1:5">
+      <c r="A71" s="1">
+        <v>44461</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="72" customHeight="1" spans="1:5">
+      <c r="A72" s="1">
+        <v>44462</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="73" customHeight="1" spans="1:5">
+      <c r="A73" s="1">
+        <v>44463</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C73" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="74" customHeight="1" spans="1:5">
+      <c r="A74" s="1">
+        <v>44466</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>258</v>
       </c>
     </row>
   </sheetData>

</xml_diff>